<commit_message>
Added Roshi's Motivation section to Final Report
References need adding and citations updated.
</commit_message>
<xml_diff>
--- a/FinalProject/data/meetings.xlsx
+++ b/FinalProject/data/meetings.xlsx
@@ -1,16 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\FinalProject\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_C2DF0B6FDA35479EAE71D8AF3C354818E41985E3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2232FADE-0878-460F-8337-E629513F3087}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -30,34 +44,46 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>Ann</t>
-  </si>
-  <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Team Formation</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Team Formation Formation Formation Formation Formation </t>
-  </si>
-  <si>
-    <t>Final Meeting</t>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Georgios</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Roshi</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>Group Formation: set up communication channel in Slack and GitHub repository</t>
+  </si>
+  <si>
+    <t>Agreed topic of "Plastic Pollution", distributed research activity for week</t>
+  </si>
+  <si>
+    <t>Presented inividuals' research findings and discussed hypothesis</t>
+  </si>
+  <si>
+    <t>Decided on final dataset to use and hypothesis of "proportion of marine plastics pollution does not change over time"</t>
+  </si>
+  <si>
+    <t>Presentation draft agreed</t>
+  </si>
+  <si>
+    <t>Distributed section writing activity for week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -96,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,16 +454,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,201 +477,241 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>43501</v>
+        <v>43866</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>43502</v>
+        <v>43872</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>43503</v>
+        <f>B3+7</f>
+        <v>43879</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>43504</v>
+        <f t="shared" ref="B5:B16" si="0">B4+7</f>
+        <v>43886</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>43505</v>
+        <v>43894</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>43506</v>
+        <v>43900</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>43507</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f t="shared" si="0"/>
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>43508</v>
-      </c>
-      <c r="C9" t="s">
+        <f t="shared" si="0"/>
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>43928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>43935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Final Report (more edits)
</commit_message>
<xml_diff>
--- a/FinalProject/data/meetings.xlsx
+++ b/FinalProject/data/meetings.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalyj\OneDrive\RGU\MSc Data Science\CMM507Group2\FinalProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7e4705127bdb922/RGU/MSc Data Science/CMM507Group2/FinalProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_C2DF0B6FDA35479EAE71D8AF3C354818E41985E3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2232FADE-0878-460F-8337-E629513F3087}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_C2DF0B6FDA35479EAE71D8AF3C354818E41985E3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F15E18DF-ABD6-4035-AE4A-D512BB6356C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="27">
   <si>
     <t>No</t>
   </si>
@@ -74,10 +74,46 @@
     <t>Decided on final dataset to use and hypothesis of "proportion of marine plastics pollution does not change over time"</t>
   </si>
   <si>
-    <t>Presentation draft agreed</t>
-  </si>
-  <si>
-    <t>Distributed section writing activity for week</t>
+    <t>Cancelled to support other modules</t>
+  </si>
+  <si>
+    <t>Cancelled due to Covid-19 arrangements</t>
+  </si>
+  <si>
+    <t>Cancelled with agreement</t>
+  </si>
+  <si>
+    <t>Presentation dry run and literature sources distributed for review</t>
+  </si>
+  <si>
+    <t>Distributed section writing activity for week and discussed predictive model</t>
+  </si>
+  <si>
+    <t>Presentation draft agreed and agreed data needed re-categorising</t>
+  </si>
+  <si>
+    <t>Agreed structure of the final report</t>
+  </si>
+  <si>
+    <t>First review of the final report</t>
+  </si>
+  <si>
+    <t>Discussed consolidated changes from first review</t>
+  </si>
+  <si>
+    <t>Reviewed coursework guidelines to ensure compliance and agreed on internal deadline</t>
+  </si>
+  <si>
+    <t>Finalised sections and identified last gaps to address</t>
+  </si>
+  <si>
+    <t>Refresh of project material and set plan for remaining time till submission</t>
+  </si>
+  <si>
+    <t>Final review and congratulations all around on a successfully completed report</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -455,18 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.69921875" customWidth="1"/>
+    <col min="1" max="1" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.875" customWidth="1"/>
+    <col min="4" max="8" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,7 +556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,7 +582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -571,12 +609,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:B16" si="0">B4+7</f>
+        <f t="shared" ref="B5:B13" si="0">B4+7</f>
         <v>43886</v>
       </c>
       <c r="C5" t="s">
@@ -598,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -606,7 +644,7 @@
         <v>43894</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -624,7 +662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -632,7 +670,7 @@
         <v>43900</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -650,7 +688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -658,8 +696,26 @@
         <f t="shared" si="0"/>
         <v>43907</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -667,8 +723,26 @@
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -676,8 +750,26 @@
         <f t="shared" si="0"/>
         <v>43921</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -685,8 +777,26 @@
         <f t="shared" si="0"/>
         <v>43928</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -694,24 +804,206 @@
         <f t="shared" si="0"/>
         <v>43935</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>43942</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
+        <v>43943</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>43956</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43959</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>43960</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43961</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43962</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>